<commit_message>
Uploading ready API code
</commit_message>
<xml_diff>
--- a/fuel_api/api_inmetro/car_data_2023_test.xlsx
+++ b/fuel_api/api_inmetro/car_data_2023_test.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Versão</t>
+          <t>Versao</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0-8V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.0-8V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.0-8V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1356,7 +1356,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2249,7 +2249,7 @@
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2284,7 +2284,7 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2319,7 +2319,7 @@
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2354,7 +2354,7 @@
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2389,7 +2389,7 @@
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2818,7 +2818,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2857,7 +2857,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3052,7 +3052,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.0 - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3169,7 +3169,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3286,7 +3286,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.8L-8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.8L-8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -3676,7 +3676,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1.0-6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3910,7 +3910,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -3988,7 +3988,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -4027,7 +4027,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>1.5-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>1.5T-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>1.5T-16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -4222,7 +4222,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -4378,7 +4378,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -4456,7 +4456,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -4495,7 +4495,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -4534,7 +4534,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -4612,7 +4612,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -4651,7 +4651,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -4807,7 +4807,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>1.5T -16V</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>1.2T - 12 V</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>1.2T - 12 V</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -5041,7 +5041,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>1.2T - 12 V</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -5076,7 +5076,7 @@
       <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -5111,7 +5111,7 @@
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -5146,7 +5146,7 @@
       <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -5181,7 +5181,7 @@
       <c r="C123" t="inlineStr"/>
       <c r="D123" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -5216,7 +5216,7 @@
       <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -5251,7 +5251,7 @@
       <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -5286,7 +5286,7 @@
       <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -5321,7 +5321,7 @@
       <c r="C127" t="inlineStr"/>
       <c r="D127" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>1.0T - 12 V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -5399,7 +5399,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>1.2T - 12 V</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -5555,7 +5555,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -5594,7 +5594,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>1.6 16V T</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>1.6 16V T</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>1.0 6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>1.0 6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>1.0 6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -5828,7 +5828,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>1.0 6V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -5867,7 +5867,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -5945,7 +5945,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>1.6 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -5984,7 +5984,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -6062,7 +6062,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>1.0 12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -6101,7 +6101,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>1.0 12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>1.0 12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -6218,7 +6218,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>1.3-16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -6257,7 +6257,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>1.0 12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -6296,7 +6296,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>1.0 12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -6335,7 +6335,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>1.0 12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>1.3-8V</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -6452,7 +6452,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -6491,7 +6491,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -6530,7 +6530,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -6569,7 +6569,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -6647,7 +6647,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -6725,7 +6725,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -6842,7 +6842,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -6920,7 +6920,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -6959,7 +6959,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -6998,7 +6998,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>1.0-12V T</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -7037,7 +7037,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -7076,7 +7076,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -7115,7 +7115,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -7154,7 +7154,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -7193,7 +7193,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -7232,7 +7232,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -7271,7 +7271,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -7310,7 +7310,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -7349,7 +7349,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -7388,7 +7388,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -7427,7 +7427,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>1.6-16V T</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -7505,7 +7505,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>1.6-16V T</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -7544,7 +7544,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -7583,7 +7583,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -7622,7 +7622,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -7661,7 +7661,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -7700,7 +7700,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>1.6-16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -7739,7 +7739,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -7817,7 +7817,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -7856,7 +7856,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -7895,7 +7895,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>1.6 - 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -7934,7 +7934,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>1.6 - 16V</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -7973,7 +7973,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -8012,7 +8012,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -8051,7 +8051,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -8090,7 +8090,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>1.0-12V</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -8129,7 +8129,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -8168,7 +8168,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -8207,7 +8207,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -8246,7 +8246,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -8285,7 +8285,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -8324,7 +8324,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -8363,7 +8363,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
@@ -8402,7 +8402,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
@@ -8519,7 +8519,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -8558,7 +8558,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>2.0-16V</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
@@ -8597,7 +8597,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -8636,7 +8636,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -8675,7 +8675,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>1.8L -8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -8714,7 +8714,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>1.8L-8V</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -8753,7 +8753,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -8792,7 +8792,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -8831,7 +8831,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -8870,7 +8870,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
@@ -8909,7 +8909,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -8948,7 +8948,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>1.3 16V T</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">

</xml_diff>